<commit_message>
added other hw configurations
</commit_message>
<xml_diff>
--- a/dtpu_configurations/only_integer8/30mhz/mxu_20x20/timing.xlsx
+++ b/dtpu_configurations/only_integer8/30mhz/mxu_20x20/timing.xlsx
@@ -119,10 +119,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="n" s="4">
-        <v>5.2977213859558105</v>
+        <v>2.1835618019104004</v>
       </c>
       <c r="C2" t="n" s="4">
-        <v>0.014442224986851215</v>
+        <v>0.01949940249323845</v>
       </c>
     </row>
   </sheetData>

</xml_diff>